<commit_message>
double server setup rfid
</commit_message>
<xml_diff>
--- a/Server/rfid-server-DBS/users.xlsx
+++ b/Server/rfid-server-DBS/users.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_3D66343E5B3014E327248FD058A490A7582067CA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{837E40B2-2333-4887-B539-E48B40630C8B}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -43,37 +44,37 @@
     <t>591EF2D4</t>
   </si>
   <si>
+    <t>bob</t>
+  </si>
+  <si>
+    <t>pass2</t>
+  </si>
+  <si>
+    <t>EA4C7814</t>
+  </si>
+  <si>
+    <t>charlie</t>
+  </si>
+  <si>
+    <t>pass3</t>
+  </si>
+  <si>
+    <t>19AF56E9</t>
+  </si>
+  <si>
+    <t>Jacobe</t>
+  </si>
+  <si>
+    <t>pass4</t>
+  </si>
+  <si>
+    <t>103|202</t>
+  </si>
+  <si>
+    <t>102|103|104</t>
+  </si>
+  <si>
     <t>101|102</t>
-  </si>
-  <si>
-    <t>bob</t>
-  </si>
-  <si>
-    <t>pass2</t>
-  </si>
-  <si>
-    <t>EA4C7814</t>
-  </si>
-  <si>
-    <t>102|103|104</t>
-  </si>
-  <si>
-    <t>charlie</t>
-  </si>
-  <si>
-    <t>pass3</t>
-  </si>
-  <si>
-    <t>19AF56E9</t>
-  </si>
-  <si>
-    <t>103|202</t>
-  </si>
-  <si>
-    <t>Jacobe</t>
-  </si>
-  <si>
-    <t>pass4</t>
   </si>
   <si>
     <t>202|204</t>
@@ -82,27 +83,27 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <sz val="11"/>
-      <name val="Arial"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <sz val="11"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -478,21 +479,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.45" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="12.19921875" customWidth="1"/>
     <col min="3" max="3" width="15.1328125" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -512,7 +513,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" ht="27" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -523,47 +524,47 @@
         <v>8</v>
       </c>
       <c r="D2" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="F2" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="D3" s="2">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F3" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" ht="27" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="D4" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>17</v>
@@ -572,15 +573,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" ht="14.25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D5" s="2">
         <v>2</v>

</xml_diff>

<commit_message>
Add stats endpoint and enhance RFID test setup
Added a /stats endpoint to the Node.js server for credential-based user data retrieval. Major improvements to Double_Server_Setup_Rfid_Test.ino: added access control, admin login, status page, and backend integration for registration and access. Updated test and server configuration files and user data spreadsheets.
</commit_message>
<xml_diff>
--- a/Server/rfid-server-DBS/users.xlsx
+++ b/Server/rfid-server-DBS/users.xlsx
@@ -1,14 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_3D66343E5B3014E327248FD058A490A7582067CA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{837E40B2-2333-4887-B539-E48B40630C8B}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -44,6 +43,9 @@
     <t>591EF2D4</t>
   </si>
   <si>
+    <t>101|102</t>
+  </si>
+  <si>
     <t>bob</t>
   </si>
   <si>
@@ -53,6 +55,9 @@
     <t>EA4C7814</t>
   </si>
   <si>
+    <t>102|103|104</t>
+  </si>
+  <si>
     <t>charlie</t>
   </si>
   <si>
@@ -62,19 +67,13 @@
     <t>19AF56E9</t>
   </si>
   <si>
+    <t>103|202</t>
+  </si>
+  <si>
     <t>Jacobe</t>
   </si>
   <si>
     <t>pass4</t>
-  </si>
-  <si>
-    <t>103|202</t>
-  </si>
-  <si>
-    <t>102|103|104</t>
-  </si>
-  <si>
-    <t>101|102</t>
   </si>
   <si>
     <t>202|204</t>
@@ -83,27 +82,27 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <color theme="1"/>
+      <family val="2"/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
+      <color theme="1"/>
+      <family val="2"/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -479,21 +478,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.45" customHeight="1"/>
   <cols>
     <col min="2" max="2" width="12.19921875" customWidth="1"/>
     <col min="3" max="3" width="15.1328125" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" ht="27.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -513,7 +512,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" ht="27" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -527,44 +526,44 @@
         <v>16</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="F2" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F3" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" ht="27" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D4" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>17</v>
@@ -573,15 +572,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" ht="14.25" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="D5" s="2">
         <v>2</v>

</xml_diff>